<commit_message>
updated the table of frequencies
</commit_message>
<xml_diff>
--- a/Frequency_Conversions.xlsx
+++ b/Frequency_Conversions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Time Wanted</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>C3-B3</t>
+  </si>
+  <si>
+    <t>Clock / Machine</t>
   </si>
 </sst>
 </file>
@@ -455,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +474,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,37 +505,32 @@
       <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4</v>
       </c>
       <c r="C2" s="3">
-        <f>(A2)/(12*(1/$J$2))</f>
-        <v>2457666.6666666665</v>
+        <f>(A2)/($N$2*(1/$J$2))</f>
+        <v>14745999.999999998</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>IF( C2 &gt; $K$2, (IF( C2 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
         <v>HUGE</v>
       </c>
       <c r="E2" s="3">
-        <f>_xlfn.FLOOR.MATH(C2/$I$2)</f>
-        <v>24576</v>
+        <f t="shared" ref="E2:E19" si="0">_xlfn.FLOOR.MATH(C2/$I$2)</f>
+        <v>65537</v>
       </c>
       <c r="F2" s="1" t="str">
         <f>IF( E2 &gt; $K$2, (IF( E2 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
-        <v>LONG</v>
-      </c>
-      <c r="G2" s="1">
-        <f>4*E2</f>
-        <v>98304</v>
-      </c>
-      <c r="H2" s="1" t="str">
-        <f>IF( G2 &gt; $K$2, (IF( G2 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
         <v>HUGE</v>
       </c>
       <c r="I2" s="1">
-        <v>100</v>
+        <v>225</v>
       </c>
       <c r="J2" s="1">
         <f>7.373*10^6</f>
@@ -547,34 +545,29 @@
       <c r="M2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
       <c r="C3" s="3">
-        <f>(A3)/(12*(1/$J$2))</f>
-        <v>1843249.9999999998</v>
+        <f t="shared" ref="C3:C19" si="1">(A3)/($N$2*(1/$J$2))</f>
+        <v>11059500</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:D19" si="0">IF( C3 &gt; $K$2, (IF( C3 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" ref="D3:D19" si="2">IF( C3 &gt; $K$2, (IF( C3 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
         <v>HUGE</v>
       </c>
       <c r="E3" s="3">
         <f>_xlfn.FLOOR.MATH(C3/$I$2)</f>
-        <v>18432</v>
+        <v>49153</v>
       </c>
       <c r="F3" s="1" t="str">
-        <f t="shared" ref="F3:F19" si="1">IF( E3 &gt; $K$2, (IF( E3 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
-        <v>LONG</v>
-      </c>
-      <c r="G3" s="1">
-        <f t="shared" ref="G3:G19" si="2">4*E3</f>
-        <v>73728</v>
-      </c>
-      <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H19" si="3">IF( G3 &gt; $K$2, (IF( G3 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
-        <v>HUGE</v>
+        <f t="shared" ref="F3:F19" si="3">IF( E3 &gt; $K$2, (IF( E3 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <v>LONG</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>28</v>
@@ -586,89 +579,65 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="C4" s="3">
-        <f>(A4)/(12*(1/$J$2))</f>
-        <v>1228833.3333333333</v>
+        <f t="shared" si="1"/>
+        <v>7372999.9999999991</v>
       </c>
       <c r="D4" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E4" s="3">
-        <f>_xlfn.FLOOR.MATH(C4/$I$2)</f>
-        <v>12288</v>
+        <v>32768</v>
       </c>
       <c r="F4" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G4" s="1">
-        <f t="shared" si="2"/>
-        <v>49152</v>
-      </c>
-      <c r="H4" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="3">
-        <f>(A5)/(12*(1/$J$2))</f>
-        <v>614416.66666666663</v>
+        <f t="shared" si="1"/>
+        <v>3686499.9999999995</v>
       </c>
       <c r="D5" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E5" s="3">
-        <f>_xlfn.FLOOR.MATH(C5/$I$2)</f>
-        <v>6144</v>
+        <v>16384</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G5" s="1">
-        <f t="shared" si="2"/>
-        <v>24576</v>
-      </c>
-      <c r="H5" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.5</v>
       </c>
       <c r="C6" s="3">
-        <f>(A6)/(12*(1/$J$2))</f>
-        <v>307208.33333333331</v>
+        <f t="shared" si="1"/>
+        <v>1843249.9999999998</v>
       </c>
       <c r="D6" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E6" s="3">
-        <f>_xlfn.FLOOR.MATH(C6/$I$2)</f>
-        <v>3072</v>
+        <v>8192</v>
       </c>
       <c r="F6" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G6" s="1">
-        <f t="shared" si="2"/>
-        <v>12288</v>
-      </c>
-      <c r="H6" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
@@ -677,384 +646,283 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.4</v>
       </c>
       <c r="C7" s="3">
-        <f>(A7)/(12*(1/$J$2))</f>
-        <v>245766.66666666666</v>
+        <f t="shared" si="1"/>
+        <v>1474600</v>
       </c>
       <c r="D7" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E7" s="3">
-        <f>_xlfn.FLOOR.MATH(C7/$I$2)</f>
-        <v>2457</v>
+        <v>6553</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" si="2"/>
-        <v>9828</v>
-      </c>
-      <c r="H7" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.2</v>
       </c>
       <c r="C8" s="3">
-        <f>(A8)/(12*(1/$J$2))</f>
-        <v>122883.33333333333</v>
+        <f t="shared" si="1"/>
+        <v>737300</v>
       </c>
       <c r="D8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E8" s="3">
-        <f>_xlfn.FLOOR.MATH(C8/$I$2)</f>
-        <v>1228</v>
+        <v>3276</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="2"/>
-        <v>4912</v>
-      </c>
-      <c r="H8" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.1</v>
       </c>
       <c r="C9" s="3">
-        <f>(A9)/(12*(1/$J$2))</f>
-        <v>61441.666666666664</v>
+        <f t="shared" si="1"/>
+        <v>368650</v>
       </c>
       <c r="D9" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E9" s="3">
         <f t="shared" si="0"/>
-        <v>LONG</v>
-      </c>
-      <c r="E9" s="3">
-        <f>_xlfn.FLOOR.MATH(C9/$I$2)</f>
-        <v>614</v>
+        <v>1638</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="2"/>
-        <v>2456</v>
-      </c>
-      <c r="H9" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.99</v>
       </c>
       <c r="C10" s="3">
-        <f>(A10)/(12*(1/$J$2))</f>
-        <v>608272.5</v>
+        <f t="shared" si="1"/>
+        <v>3649634.9999999995</v>
       </c>
       <c r="D10" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E10" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E10" s="3">
-        <f>_xlfn.FLOOR.MATH(C10/$I$2)</f>
-        <v>6082</v>
+        <v>16220</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G10" s="1">
-        <f t="shared" si="2"/>
-        <v>24328</v>
-      </c>
-      <c r="H10" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1.99</v>
       </c>
       <c r="C11" s="3">
-        <f>(A11)/(12*(1/$J$2))</f>
-        <v>1222689.1666666665</v>
+        <f t="shared" si="1"/>
+        <v>7336134.9999999991</v>
       </c>
       <c r="D11" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E11" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E11" s="3">
-        <f>_xlfn.FLOOR.MATH(C11/$I$2)</f>
-        <v>12226</v>
+        <v>32605</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G11" s="1">
-        <f t="shared" si="2"/>
-        <v>48904</v>
-      </c>
-      <c r="H11" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2.99</v>
       </c>
       <c r="C12" s="3">
-        <f>(A12)/(12*(1/$J$2))</f>
-        <v>1837105.8333333333</v>
+        <f t="shared" si="1"/>
+        <v>11022635</v>
       </c>
       <c r="D12" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E12" s="3">
-        <f>_xlfn.FLOOR.MATH(C12/$I$2)</f>
-        <v>18371</v>
+        <v>48989</v>
       </c>
       <c r="F12" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G12" s="1">
-        <f t="shared" si="2"/>
-        <v>73484</v>
-      </c>
-      <c r="H12" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>HUGE</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>3.99</v>
       </c>
       <c r="C13" s="3">
-        <f>(A13)/(12*(1/$J$2))</f>
-        <v>2451522.5</v>
+        <f t="shared" si="1"/>
+        <v>14709135</v>
       </c>
       <c r="D13" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E13" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E13" s="3">
-        <f>_xlfn.FLOOR.MATH(C13/$I$2)</f>
-        <v>24515</v>
+        <v>65373</v>
       </c>
       <c r="F13" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G13" s="1">
-        <f t="shared" si="2"/>
-        <v>98060</v>
-      </c>
-      <c r="H13" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>HUGE</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.01</v>
       </c>
       <c r="C14" s="3">
-        <f>(A14)/(12*(1/$J$2))</f>
-        <v>6144.1666666666661</v>
+        <f t="shared" si="1"/>
+        <v>36865</v>
       </c>
       <c r="D14" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>LONG</v>
+      </c>
+      <c r="E14" s="3">
         <f t="shared" si="0"/>
-        <v>LONG</v>
-      </c>
-      <c r="E14" s="3">
-        <f>_xlfn.FLOOR.MATH(C14/$I$2)</f>
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="F14" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SMALL</v>
-      </c>
-      <c r="G14" s="1">
-        <f t="shared" si="2"/>
-        <v>244</v>
-      </c>
-      <c r="H14" s="1" t="str">
         <f t="shared" si="3"/>
         <v>SMALL</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C15" s="3">
-        <f>(A15)/(12*(1/$J$2))</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D15" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>SMALL</v>
+      </c>
+      <c r="E15" s="3">
         <f t="shared" si="0"/>
-        <v>SMALL</v>
-      </c>
-      <c r="E15" s="3">
-        <f>_xlfn.FLOOR.MATH(C15/$I$2)</f>
         <v>0</v>
       </c>
       <c r="F15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>SMALL</v>
-      </c>
-      <c r="G15" s="1">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="str">
         <f t="shared" si="3"/>
         <v>SMALL</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>1.99</v>
       </c>
       <c r="C16" s="3">
-        <f>(A16)/(12*(1/$J$2))</f>
-        <v>1222689.1666666665</v>
+        <f t="shared" si="1"/>
+        <v>7336134.9999999991</v>
       </c>
       <c r="D16" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E16" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E16" s="3">
-        <f>_xlfn.FLOOR.MATH(C16/$I$2)</f>
-        <v>12226</v>
+        <v>32605</v>
       </c>
       <c r="F16" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G16" s="1">
-        <f t="shared" si="2"/>
-        <v>48904</v>
-      </c>
-      <c r="H16" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.99</v>
       </c>
-      <c r="C17" s="1">
-        <f>(A17)/(12*(1/$J$2))</f>
-        <v>608272.5</v>
+      <c r="C17" s="3">
+        <f t="shared" si="1"/>
+        <v>3649634.9999999995</v>
       </c>
       <c r="D17" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E17" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E17" s="1">
-        <f>_xlfn.FLOOR.MATH(C17/$I$2)</f>
-        <v>6082</v>
+        <v>16220</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G17" s="1">
-        <f t="shared" si="2"/>
-        <v>24328</v>
-      </c>
-      <c r="H17" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.49</v>
       </c>
-      <c r="C18" s="1">
-        <f>(A18)/(12*(1/$J$2))</f>
-        <v>301064.16666666663</v>
+      <c r="C18" s="3">
+        <f t="shared" si="1"/>
+        <v>1806384.9999999998</v>
       </c>
       <c r="D18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>HUGE</v>
+      </c>
+      <c r="E18" s="3">
         <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E18" s="1">
-        <f>_xlfn.FLOOR.MATH(C18/$I$2)</f>
-        <v>3010</v>
+        <v>8028</v>
       </c>
       <c r="F18" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="C19" s="3">
         <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G18" s="1">
+        <v>884759.99999999988</v>
+      </c>
+      <c r="D19" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12040</v>
-      </c>
-      <c r="H18" s="1" t="str">
+        <v>HUGE</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>3932</v>
+      </c>
+      <c r="F19" s="1" t="str">
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.249</v>
-      </c>
-      <c r="C19" s="1">
-        <f>(A19)/(12*(1/$J$2))</f>
-        <v>152989.75</v>
-      </c>
-      <c r="D19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>HUGE</v>
-      </c>
-      <c r="E19" s="1">
-        <f>_xlfn.FLOOR.MATH(C19/$I$2)</f>
-        <v>1529</v>
-      </c>
-      <c r="F19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>LONG</v>
-      </c>
-      <c r="G19" s="1">
-        <f t="shared" si="2"/>
-        <v>6116</v>
-      </c>
-      <c r="H19" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>LONG</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1065,7 +933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -1085,7 +953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -1093,8 +961,8 @@
         <v>261.63</v>
       </c>
       <c r="C26" s="3">
-        <f>(1/B26)/(12*(1/$J$2))</f>
-        <v>2348.4182496910394</v>
+        <f>(1/B26)/($N$2*(1/$J$2))</f>
+        <v>14090.509498146235</v>
       </c>
       <c r="D26" s="1" t="str">
         <f>IF( C26 &gt; $K$2, (IF( C26 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
@@ -1102,7 +970,7 @@
       </c>
       <c r="E26" s="1">
         <f>_xlfn.FLOOR.MATH(C26)</f>
-        <v>2348</v>
+        <v>14090</v>
       </c>
       <c r="F26" s="1" t="str">
         <f>IF( E26 &gt; $K$2, (IF( E26 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
@@ -1112,7 +980,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -1120,23 +988,23 @@
         <v>277.18</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" ref="C27:C50" si="4">(1/B27)/(12*(1/$J$2))</f>
-        <v>2216.6702744305744</v>
+        <f t="shared" ref="C27:C50" si="4">(1/B27)/($N$2*(1/$J$2))</f>
+        <v>13300.021646583446</v>
       </c>
       <c r="D27" s="1" t="str">
-        <f t="shared" ref="D27:D50" si="5">IF( C27 &gt; $K$2, (IF( C27 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" ref="D27:D37" si="5">IF( C27 &gt; $K$2, (IF( C27 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
         <v>LONG</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" ref="E27:E38" si="6">_xlfn.FLOOR.MATH(C27)</f>
-        <v>2216</v>
+        <f t="shared" ref="E27:E37" si="6">_xlfn.FLOOR.MATH(C27)</f>
+        <v>13300</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f t="shared" ref="F27:F50" si="7">IF( E27 &gt; $K$2, (IF( E27 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
-        <v>LONG</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F27:F37" si="7">IF( E27 &gt; $K$2, (IF( E27 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
@@ -1145,7 +1013,7 @@
       </c>
       <c r="C28" s="3">
         <f t="shared" si="4"/>
-        <v>2092.2722422756474</v>
+        <v>12553.633453653883</v>
       </c>
       <c r="D28" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1153,14 +1021,14 @@
       </c>
       <c r="E28" s="1">
         <f t="shared" si="6"/>
-        <v>2092</v>
+        <v>12553</v>
       </c>
       <c r="F28" s="1" t="str">
         <f t="shared" si="7"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -1169,7 +1037,7 @@
       </c>
       <c r="C29" s="3">
         <f t="shared" si="4"/>
-        <v>1974.7908162718691</v>
+        <v>11848.744897631215</v>
       </c>
       <c r="D29" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1177,14 +1045,14 @@
       </c>
       <c r="E29" s="1">
         <f t="shared" si="6"/>
-        <v>1974</v>
+        <v>11848</v>
       </c>
       <c r="F29" s="1" t="str">
         <f t="shared" si="7"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1193,7 +1061,7 @@
       </c>
       <c r="C30" s="3">
         <f t="shared" si="4"/>
-        <v>1863.9585798218202</v>
+        <v>11183.751478930921</v>
       </c>
       <c r="D30" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1201,14 +1069,14 @@
       </c>
       <c r="E30" s="1">
         <f t="shared" si="6"/>
-        <v>1863</v>
+        <v>11183</v>
       </c>
       <c r="F30" s="1" t="str">
         <f t="shared" si="7"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
@@ -1217,7 +1085,7 @@
       </c>
       <c r="C31" s="3">
         <f t="shared" si="4"/>
-        <v>1759.346753333524</v>
+        <v>10556.080520001144</v>
       </c>
       <c r="D31" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1225,14 +1093,14 @@
       </c>
       <c r="E31" s="1">
         <f t="shared" si="6"/>
-        <v>1759</v>
+        <v>10556</v>
       </c>
       <c r="F31" s="1" t="str">
         <f t="shared" si="7"/>
         <v>LONG</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -1241,7 +1109,7 @@
       </c>
       <c r="C32" s="3">
         <f t="shared" si="4"/>
-        <v>1660.6304674901123</v>
+        <v>9963.7828049406726</v>
       </c>
       <c r="D32" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1249,7 +1117,7 @@
       </c>
       <c r="E32" s="1">
         <f t="shared" si="6"/>
-        <v>1660</v>
+        <v>9963</v>
       </c>
       <c r="F32" s="1" t="str">
         <f t="shared" si="7"/>
@@ -1265,7 +1133,7 @@
       </c>
       <c r="C33" s="3">
         <f t="shared" si="4"/>
-        <v>1567.3894557823128</v>
+        <v>9404.3367346938758</v>
       </c>
       <c r="D33" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1273,7 +1141,7 @@
       </c>
       <c r="E33" s="1">
         <f t="shared" si="6"/>
-        <v>1567</v>
+        <v>9404</v>
       </c>
       <c r="F33" s="1" t="str">
         <f t="shared" si="7"/>
@@ -1289,7 +1157,7 @@
       </c>
       <c r="C34" s="3">
         <f t="shared" si="4"/>
-        <v>1479.4526045429006</v>
+        <v>8876.715627257403</v>
       </c>
       <c r="D34" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1297,7 +1165,7 @@
       </c>
       <c r="E34" s="1">
         <f t="shared" si="6"/>
-        <v>1479</v>
+        <v>8876</v>
       </c>
       <c r="F34" s="1" t="str">
         <f t="shared" si="7"/>
@@ -1313,7 +1181,7 @@
       </c>
       <c r="C35" s="3">
         <f t="shared" si="4"/>
-        <v>1396.401515151515</v>
+        <v>8378.4090909090901</v>
       </c>
       <c r="D35" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1321,7 +1189,7 @@
       </c>
       <c r="E35" s="1">
         <f t="shared" si="6"/>
-        <v>1396</v>
+        <v>8378</v>
       </c>
       <c r="F35" s="1" t="str">
         <f t="shared" si="7"/>
@@ -1337,7 +1205,7 @@
       </c>
       <c r="C36" s="3">
         <f t="shared" si="4"/>
-        <v>1318.0381557119156</v>
+        <v>7908.2289342714939</v>
       </c>
       <c r="D36" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1345,7 +1213,7 @@
       </c>
       <c r="E36" s="1">
         <f t="shared" si="6"/>
-        <v>1318</v>
+        <v>7908</v>
       </c>
       <c r="F36" s="1" t="str">
         <f t="shared" si="7"/>
@@ -1361,7 +1229,7 @@
       </c>
       <c r="C37" s="3">
         <f t="shared" si="4"/>
-        <v>1244.0606355120003</v>
+        <v>7464.3638130720019</v>
       </c>
       <c r="D37" s="1" t="str">
         <f t="shared" si="5"/>
@@ -1369,7 +1237,7 @@
       </c>
       <c r="E37" s="1">
         <f t="shared" si="6"/>
-        <v>1244</v>
+        <v>7464</v>
       </c>
       <c r="F37" s="1" t="str">
         <f t="shared" si="7"/>
@@ -1384,8 +1252,8 @@
         <v>523.25</v>
       </c>
       <c r="C38" s="3">
-        <f>(1/B38)/(12*(1/$J$2))</f>
-        <v>1174.2315655359132</v>
+        <f t="shared" si="4"/>
+        <v>7045.3893932154797</v>
       </c>
       <c r="D38" s="1" t="str">
         <f>IF( C38 &gt; $K$2, (IF( C38 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
@@ -1393,7 +1261,7 @@
       </c>
       <c r="E38" s="1">
         <f>_xlfn.FLOOR.MATH(C38)</f>
-        <v>1174</v>
+        <v>7045</v>
       </c>
       <c r="F38" s="1" t="str">
         <f>IF( E38 &gt; $K$2, (IF( E38 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
@@ -1404,6 +1272,7 @@
       <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -1413,19 +1282,19 @@
         <v>130.81</v>
       </c>
       <c r="C40" s="3">
-        <f>(1/B40)/(12*(1/$J$2))</f>
-        <v>4697.0160283362629</v>
+        <f t="shared" si="4"/>
+        <v>28182.096170017579</v>
       </c>
       <c r="D40" s="1" t="str">
-        <f>IF( C40 &gt; $K$2, (IF( C40 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" ref="D40:D51" si="8">IF( C40 &gt; $K$2, (IF( C40 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
         <v>LONG</v>
       </c>
       <c r="E40" s="1">
-        <f t="shared" ref="E40:E51" si="8">_xlfn.FLOOR.MATH(C40)</f>
-        <v>4697</v>
+        <f t="shared" ref="E40:E51" si="9">_xlfn.FLOOR.MATH(C40)</f>
+        <v>28182</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f>IF( E40 &gt; $K$2, (IF( E40 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" ref="F40:F51" si="10">IF( E40 &gt; $K$2, (IF( E40 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
         <v>LONG</v>
       </c>
     </row>
@@ -1437,19 +1306,19 @@
         <v>138.59</v>
       </c>
       <c r="C41" s="3">
-        <f>(1/B41)/(12*(1/$J$2))</f>
-        <v>4433.3405488611488</v>
+        <f t="shared" si="4"/>
+        <v>26600.043293166891</v>
       </c>
       <c r="D41" s="1" t="str">
-        <f>IF( C41 &gt; $K$2, (IF( C41 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E41" s="1">
-        <f t="shared" si="8"/>
-        <v>4433</v>
+        <f t="shared" si="9"/>
+        <v>26600</v>
       </c>
       <c r="F41" s="1" t="str">
-        <f>IF( E41 &gt; $K$2, (IF( E41 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1461,19 +1330,19 @@
         <v>146.83000000000001</v>
       </c>
       <c r="C42" s="3">
-        <f>(1/B42)/(12*(1/$J$2))</f>
-        <v>4184.5444845512948</v>
+        <f t="shared" si="4"/>
+        <v>25107.266907307767</v>
       </c>
       <c r="D42" s="1" t="str">
-        <f>IF( C42 &gt; $K$2, (IF( C42 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E42" s="1">
-        <f t="shared" si="8"/>
-        <v>4184</v>
+        <f t="shared" si="9"/>
+        <v>25107</v>
       </c>
       <c r="F42" s="1" t="str">
-        <f>IF( E42 &gt; $K$2, (IF( E42 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1485,19 +1354,19 @@
         <v>155.56</v>
       </c>
       <c r="C43" s="3">
-        <f>(1/B43)/(12*(1/$J$2))</f>
-        <v>3949.7085797548639</v>
+        <f t="shared" si="4"/>
+        <v>23698.251478529182</v>
       </c>
       <c r="D43" s="1" t="str">
-        <f>IF( C43 &gt; $K$2, (IF( C43 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E43" s="1">
-        <f t="shared" si="8"/>
-        <v>3949</v>
+        <f t="shared" si="9"/>
+        <v>23698</v>
       </c>
       <c r="F43" s="1" t="str">
-        <f>IF( E43 &gt; $K$2, (IF( E43 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1509,19 +1378,19 @@
         <v>164.81</v>
       </c>
       <c r="C44" s="3">
-        <f>(1/B44)/(12*(1/$J$2))</f>
-        <v>3728.0302570636891</v>
+        <f t="shared" si="4"/>
+        <v>22368.181542382135</v>
       </c>
       <c r="D44" s="1" t="str">
-        <f>IF( C44 &gt; $K$2, (IF( C44 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E44" s="1">
-        <f t="shared" si="8"/>
-        <v>3728</v>
+        <f t="shared" si="9"/>
+        <v>22368</v>
       </c>
       <c r="F44" s="1" t="str">
-        <f>IF( E44 &gt; $K$2, (IF( E44 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1533,19 +1402,19 @@
         <v>174.61</v>
       </c>
       <c r="C45" s="3">
-        <f>(1/B45)/(12*(1/$J$2))</f>
-        <v>3518.7942653150826</v>
+        <f t="shared" si="4"/>
+        <v>21112.765591890497</v>
       </c>
       <c r="D45" s="1" t="str">
-        <f>IF( C45 &gt; $K$2, (IF( C45 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="8"/>
-        <v>3518</v>
+        <f t="shared" si="9"/>
+        <v>21112</v>
       </c>
       <c r="F45" s="1" t="str">
-        <f>IF( E45 &gt; $K$2, (IF( E45 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1557,19 +1426,19 @@
         <v>185</v>
       </c>
       <c r="C46" s="3">
-        <f>(1/B46)/(12*(1/$J$2))</f>
-        <v>3321.171171171171</v>
+        <f t="shared" si="4"/>
+        <v>19927.027027027027</v>
       </c>
       <c r="D46" s="1" t="str">
-        <f>IF( C46 &gt; $K$2, (IF( C46 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E46" s="1">
-        <f t="shared" si="8"/>
-        <v>3321</v>
+        <f t="shared" si="9"/>
+        <v>19927</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f>IF( E46 &gt; $K$2, (IF( E46 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1581,19 +1450,19 @@
         <v>196</v>
       </c>
       <c r="C47" s="3">
-        <f>(1/B47)/(12*(1/$J$2))</f>
-        <v>3134.7789115646256</v>
+        <f t="shared" si="4"/>
+        <v>18808.673469387752</v>
       </c>
       <c r="D47" s="1" t="str">
-        <f>IF( C47 &gt; $K$2, (IF( C47 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" si="8"/>
-        <v>3134</v>
+        <f t="shared" si="9"/>
+        <v>18808</v>
       </c>
       <c r="F47" s="1" t="str">
-        <f>IF( E47 &gt; $K$2, (IF( E47 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1605,19 +1474,19 @@
         <v>207.65</v>
       </c>
       <c r="C48" s="3">
-        <f>(1/B48)/(12*(1/$J$2))</f>
-        <v>2958.9052090858013</v>
+        <f t="shared" si="4"/>
+        <v>17753.431254514806</v>
       </c>
       <c r="D48" s="1" t="str">
-        <f>IF( C48 &gt; $K$2, (IF( C48 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E48" s="1">
-        <f t="shared" si="8"/>
-        <v>2958</v>
+        <f t="shared" si="9"/>
+        <v>17753</v>
       </c>
       <c r="F48" s="1" t="str">
-        <f>IF( E48 &gt; $K$2, (IF( E48 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1629,19 +1498,19 @@
         <v>220</v>
       </c>
       <c r="C49" s="3">
-        <f>(1/B49)/(12*(1/$J$2))</f>
-        <v>2792.80303030303</v>
+        <f t="shared" si="4"/>
+        <v>16756.81818181818</v>
       </c>
       <c r="D49" s="1" t="str">
-        <f>IF( C49 &gt; $K$2, (IF( C49 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E49" s="1">
-        <f t="shared" si="8"/>
-        <v>2792</v>
+        <f t="shared" si="9"/>
+        <v>16756</v>
       </c>
       <c r="F49" s="1" t="str">
-        <f>IF( E49 &gt; $K$2, (IF( E49 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1653,19 +1522,19 @@
         <v>233.08</v>
       </c>
       <c r="C50" s="3">
-        <f>(1/B50)/(12*(1/$J$2))</f>
-        <v>2636.0763114238312</v>
+        <f t="shared" si="4"/>
+        <v>15816.457868542988</v>
       </c>
       <c r="D50" s="1" t="str">
-        <f>IF( C50 &gt; $K$2, (IF( C50 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E50" s="1">
-        <f t="shared" si="8"/>
-        <v>2636</v>
+        <f t="shared" si="9"/>
+        <v>15816</v>
       </c>
       <c r="F50" s="1" t="str">
-        <f>IF( E50 &gt; $K$2, (IF( E50 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1677,19 +1546,19 @@
         <v>246.94</v>
       </c>
       <c r="C51" s="3">
-        <f>(1/B51)/(12*(1/$J$2))</f>
-        <v>2488.1212710240006</v>
+        <f>(1/B51)/($N$2*(1/$J$2))</f>
+        <v>14928.727626144004</v>
       </c>
       <c r="D51" s="1" t="str">
-        <f>IF( C51 &gt; $K$2, (IF( C51 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E51" s="1">
-        <f t="shared" si="8"/>
-        <v>2488</v>
+        <f t="shared" si="9"/>
+        <v>14928</v>
       </c>
       <c r="F51" s="1" t="str">
-        <f>IF( E51 &gt; $K$2, (IF( E51 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added breadboard stuff and implemented the keyboard feature.
</commit_message>
<xml_diff>
--- a/Frequency_Conversions.xlsx
+++ b/Frequency_Conversions.xlsx
@@ -460,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
made some changes and tested some things. Something doesn't seem right
</commit_message>
<xml_diff>
--- a/Frequency_Conversions.xlsx
+++ b/Frequency_Conversions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CPE-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CPE-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB342DB-3A06-4949-B99A-F177C5481F0B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -134,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -457,11 +458,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,10 +642,6 @@
         <f t="shared" si="3"/>
         <v>LONG</v>
       </c>
-      <c r="J6" s="1">
-        <f>100/4</f>
-        <v>25</v>
-      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">

</xml_diff>

<commit_message>
added another frequency of notes
</commit_message>
<xml_diff>
--- a/Frequency_Conversions.xlsx
+++ b/Frequency_Conversions.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CPE-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CPE-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB342DB-3A06-4949-B99A-F177C5481F0B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Time Wanted</t>
   </si>
@@ -90,9 +89,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>C4-C5</t>
-  </si>
-  <si>
     <t>N(floored)</t>
   </si>
   <si>
@@ -102,9 +98,6 @@
     <t>FOUND AT:</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>&gt; 16 bit</t>
   </si>
   <si>
@@ -126,20 +119,28 @@
     <t>SHRINKING</t>
   </si>
   <si>
-    <t>C3-B3</t>
-  </si>
-  <si>
     <t>Clock / Machine</t>
+  </si>
+  <si>
+    <t>C4-B6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -162,10 +163,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,8 +181,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -458,11 +464,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,13 +492,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
@@ -504,10 +510,10 @@
         <v>5</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -544,7 +550,7 @@
         <v>65535</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="N2" s="1">
         <v>2</v>
@@ -571,13 +577,13 @@
         <v>LONG</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -850,7 +856,7 @@
         <v>LONG</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.99</v>
       </c>
@@ -871,7 +877,7 @@
         <v>LONG</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.49</v>
       </c>
@@ -892,7 +898,7 @@
         <v>LONG</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0.24</v>
       </c>
@@ -913,24 +919,24 @@
         <v>LONG</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E20" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -944,13 +950,13 @@
         <v>1</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -962,22 +968,19 @@
         <v>14090.509498146235</v>
       </c>
       <c r="D26" s="1" t="str">
-        <f>IF( C26 &gt; $K$2, (IF( C26 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" ref="D26" si="4">IF( C26 &gt; $K$2, (IF( C26 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
         <v>LONG</v>
       </c>
       <c r="E26" s="1">
-        <f>_xlfn.FLOOR.MATH(C26)</f>
+        <f t="shared" ref="E26" si="5">_xlfn.FLOOR.MATH(C26)</f>
         <v>14090</v>
       </c>
       <c r="F26" s="1" t="str">
-        <f>IF( E26 &gt; $K$2, (IF( E26 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
-        <v>LONG</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F26" si="6">IF( E26 &gt; $K$2, (IF( E26 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>10</v>
       </c>
@@ -985,23 +988,23 @@
         <v>277.18</v>
       </c>
       <c r="C27" s="3">
-        <f t="shared" ref="C27:C50" si="4">(1/B27)/($N$2*(1/$J$2))</f>
+        <f t="shared" ref="C27:C61" si="7">(1/B27)/($N$2*(1/$J$2))</f>
         <v>13300.021646583446</v>
       </c>
       <c r="D27" s="1" t="str">
-        <f t="shared" ref="D27:D37" si="5">IF( C27 &gt; $K$2, (IF( C27 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" ref="D27:D61" si="8">IF( C27 &gt; $K$2, (IF( C27 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
         <v>LONG</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" ref="E27:E37" si="6">_xlfn.FLOOR.MATH(C27)</f>
+        <f t="shared" ref="E27:E61" si="9">_xlfn.FLOOR.MATH(C27)</f>
         <v>13300</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f t="shared" ref="F27:F37" si="7">IF( E27 &gt; $K$2, (IF( E27 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
-        <v>LONG</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F27:F61" si="10">IF( E27 &gt; $K$2, (IF( E27 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
@@ -1009,23 +1012,23 @@
         <v>293.66000000000003</v>
       </c>
       <c r="C28" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>12553.633453653883</v>
       </c>
       <c r="D28" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>12553</v>
       </c>
       <c r="F28" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>LONG</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -1033,23 +1036,23 @@
         <v>311.13</v>
       </c>
       <c r="C29" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>11848.744897631215</v>
       </c>
       <c r="D29" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>11848</v>
       </c>
       <c r="F29" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>LONG</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -1057,23 +1060,23 @@
         <v>329.63</v>
       </c>
       <c r="C30" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>11183.751478930921</v>
       </c>
       <c r="D30" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>11183</v>
       </c>
       <c r="F30" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>LONG</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
@@ -1081,23 +1084,23 @@
         <v>349.23</v>
       </c>
       <c r="C31" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>10556.080520001144</v>
       </c>
       <c r="D31" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10556</v>
       </c>
       <c r="F31" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>LONG</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -1105,19 +1108,19 @@
         <v>369.99</v>
       </c>
       <c r="C32" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9963.7828049406726</v>
       </c>
       <c r="D32" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9963</v>
       </c>
       <c r="F32" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1129,19 +1132,19 @@
         <v>392</v>
       </c>
       <c r="C33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>9404.3367346938758</v>
       </c>
       <c r="D33" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9404</v>
       </c>
       <c r="F33" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1153,19 +1156,19 @@
         <v>415.3</v>
       </c>
       <c r="C34" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8876.715627257403</v>
       </c>
       <c r="D34" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>8876</v>
       </c>
       <c r="F34" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1177,19 +1180,19 @@
         <v>440</v>
       </c>
       <c r="C35" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>8378.4090909090901</v>
       </c>
       <c r="D35" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>8378</v>
       </c>
       <c r="F35" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1201,19 +1204,19 @@
         <v>466.16</v>
       </c>
       <c r="C36" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7908.2289342714939</v>
       </c>
       <c r="D36" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E36" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>7908</v>
       </c>
       <c r="F36" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1225,19 +1228,19 @@
         <v>493.88</v>
       </c>
       <c r="C37" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7464.3638130720019</v>
       </c>
       <c r="D37" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E37" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>7464</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
@@ -1249,62 +1252,80 @@
         <v>523.25</v>
       </c>
       <c r="C38" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>7045.3893932154797</v>
       </c>
       <c r="D38" s="1" t="str">
-        <f>IF( C38 &gt; $K$2, (IF( C38 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E38" s="1">
-        <f>_xlfn.FLOOR.MATH(C38)</f>
+        <f t="shared" si="9"/>
         <v>7045</v>
       </c>
       <c r="F38" s="1" t="str">
-        <f>IF( E38 &gt; $K$2, (IF( E38 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B39" s="4">
+        <v>554.37</v>
+      </c>
+      <c r="C39" s="3">
+        <f t="shared" si="7"/>
+        <v>6649.8908671104136</v>
+      </c>
+      <c r="D39" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E39" s="1">
+        <f t="shared" si="9"/>
+        <v>6649</v>
+      </c>
+      <c r="F39" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B40" s="4">
-        <v>130.81</v>
+        <v>587.33000000000004</v>
       </c>
       <c r="C40" s="3">
-        <f t="shared" si="4"/>
-        <v>28182.096170017579</v>
+        <f t="shared" si="7"/>
+        <v>6276.709856469105</v>
       </c>
       <c r="D40" s="1" t="str">
-        <f t="shared" ref="D40:D51" si="8">IF( C40 &gt; $K$2, (IF( C40 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="8"/>
         <v>LONG</v>
       </c>
       <c r="E40" s="1">
-        <f t="shared" ref="E40:E51" si="9">_xlfn.FLOOR.MATH(C40)</f>
-        <v>28182</v>
+        <f t="shared" si="9"/>
+        <v>6276</v>
       </c>
       <c r="F40" s="1" t="str">
-        <f t="shared" ref="F40:F51" si="10">IF( E40 &gt; $K$2, (IF( E40 &gt; $L$2, $M$3, $L$3)), $K$3)</f>
+        <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B41" s="4">
-        <v>138.59</v>
+        <v>622.25</v>
       </c>
       <c r="C41" s="3">
-        <f t="shared" si="4"/>
-        <v>26600.043293166891</v>
+        <f t="shared" si="7"/>
+        <v>5924.4676576938527</v>
       </c>
       <c r="D41" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1312,7 +1333,7 @@
       </c>
       <c r="E41" s="1">
         <f t="shared" si="9"/>
-        <v>26600</v>
+        <v>5924</v>
       </c>
       <c r="F41" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1321,14 +1342,14 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B42" s="4">
-        <v>146.83000000000001</v>
+        <v>659.25</v>
       </c>
       <c r="C42" s="3">
-        <f t="shared" si="4"/>
-        <v>25107.266907307767</v>
+        <f t="shared" si="7"/>
+        <v>5591.9605612438372</v>
       </c>
       <c r="D42" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1336,7 +1357,7 @@
       </c>
       <c r="E42" s="1">
         <f t="shared" si="9"/>
-        <v>25107</v>
+        <v>5591</v>
       </c>
       <c r="F42" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1345,14 +1366,14 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B43" s="4">
-        <v>155.56</v>
+        <v>698.46</v>
       </c>
       <c r="C43" s="3">
-        <f t="shared" si="4"/>
-        <v>23698.251478529182</v>
+        <f t="shared" si="7"/>
+        <v>5278.0402600005718</v>
       </c>
       <c r="D43" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1360,7 +1381,7 @@
       </c>
       <c r="E43" s="1">
         <f t="shared" si="9"/>
-        <v>23698</v>
+        <v>5278</v>
       </c>
       <c r="F43" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1369,14 +1390,14 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B44" s="4">
-        <v>164.81</v>
+        <v>739.99</v>
       </c>
       <c r="C44" s="3">
-        <f t="shared" si="4"/>
-        <v>22368.181542382135</v>
+        <f t="shared" si="7"/>
+        <v>4981.8240787037657</v>
       </c>
       <c r="D44" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1384,7 +1405,7 @@
       </c>
       <c r="E44" s="1">
         <f t="shared" si="9"/>
-        <v>22368</v>
+        <v>4981</v>
       </c>
       <c r="F44" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1393,14 +1414,14 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B45" s="4">
-        <v>174.61</v>
+        <v>783.99</v>
       </c>
       <c r="C45" s="3">
-        <f t="shared" si="4"/>
-        <v>21112.765591890497</v>
+        <f t="shared" si="7"/>
+        <v>4702.2283447492955</v>
       </c>
       <c r="D45" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1408,7 +1429,7 @@
       </c>
       <c r="E45" s="1">
         <f t="shared" si="9"/>
-        <v>21112</v>
+        <v>4702</v>
       </c>
       <c r="F45" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1417,14 +1438,14 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B46" s="4">
-        <v>185</v>
+        <v>830.61</v>
       </c>
       <c r="C46" s="3">
-        <f t="shared" si="4"/>
-        <v>19927.027027027027</v>
+        <f t="shared" si="7"/>
+        <v>4438.3043787096231</v>
       </c>
       <c r="D46" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1432,7 +1453,7 @@
       </c>
       <c r="E46" s="1">
         <f t="shared" si="9"/>
-        <v>19927</v>
+        <v>4438</v>
       </c>
       <c r="F46" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1441,14 +1462,14 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B47" s="4">
-        <v>196</v>
+        <v>880</v>
       </c>
       <c r="C47" s="3">
-        <f t="shared" si="4"/>
-        <v>18808.673469387752</v>
+        <f t="shared" si="7"/>
+        <v>4189.204545454545</v>
       </c>
       <c r="D47" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1456,7 +1477,7 @@
       </c>
       <c r="E47" s="1">
         <f t="shared" si="9"/>
-        <v>18808</v>
+        <v>4189</v>
       </c>
       <c r="F47" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1465,14 +1486,14 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B48" s="4">
-        <v>207.65</v>
+        <v>932.33</v>
       </c>
       <c r="C48" s="3">
-        <f t="shared" si="4"/>
-        <v>17753.431254514806</v>
+        <f t="shared" si="7"/>
+        <v>3954.0720560316622</v>
       </c>
       <c r="D48" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1480,7 +1501,7 @@
       </c>
       <c r="E48" s="1">
         <f t="shared" si="9"/>
-        <v>17753</v>
+        <v>3954</v>
       </c>
       <c r="F48" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1489,14 +1510,14 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B49" s="4">
-        <v>220</v>
+        <v>987.77</v>
       </c>
       <c r="C49" s="3">
-        <f t="shared" si="4"/>
-        <v>16756.81818181818</v>
+        <f t="shared" si="7"/>
+        <v>3732.144122619638</v>
       </c>
       <c r="D49" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1504,7 +1525,7 @@
       </c>
       <c r="E49" s="1">
         <f t="shared" si="9"/>
-        <v>16756</v>
+        <v>3732</v>
       </c>
       <c r="F49" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1513,14 +1534,14 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B50" s="4">
-        <v>233.08</v>
+        <v>1046.5</v>
       </c>
       <c r="C50" s="3">
-        <f t="shared" si="4"/>
-        <v>15816.457868542988</v>
+        <f t="shared" si="7"/>
+        <v>3522.6946966077398</v>
       </c>
       <c r="D50" s="1" t="str">
         <f t="shared" si="8"/>
@@ -1528,7 +1549,7 @@
       </c>
       <c r="E50" s="1">
         <f t="shared" si="9"/>
-        <v>15816</v>
+        <v>3522</v>
       </c>
       <c r="F50" s="1" t="str">
         <f t="shared" si="10"/>
@@ -1537,30 +1558,273 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="4">
+        <v>1108.73</v>
+      </c>
+      <c r="C51" s="3">
+        <f t="shared" si="7"/>
+        <v>3324.9754223300533</v>
+      </c>
+      <c r="D51" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E51" s="1">
+        <f t="shared" si="9"/>
+        <v>3324</v>
+      </c>
+      <c r="F51" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="4">
+        <v>1174.6600000000001</v>
+      </c>
+      <c r="C52" s="3">
+        <f t="shared" si="7"/>
+        <v>3138.3549282345525</v>
+      </c>
+      <c r="D52" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E52" s="1">
+        <f t="shared" si="9"/>
+        <v>3138</v>
+      </c>
+      <c r="F52" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="4">
+        <v>1244.51</v>
+      </c>
+      <c r="C53" s="3">
+        <f t="shared" si="7"/>
+        <v>2962.210026436107</v>
+      </c>
+      <c r="D53" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E53" s="1">
+        <f t="shared" si="9"/>
+        <v>2962</v>
+      </c>
+      <c r="F53" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="4">
+        <v>1318.51</v>
+      </c>
+      <c r="C54" s="3">
+        <f t="shared" si="7"/>
+        <v>2795.9590750164957</v>
+      </c>
+      <c r="D54" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E54" s="1">
+        <f t="shared" si="9"/>
+        <v>2795</v>
+      </c>
+      <c r="F54" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B55" s="4">
+        <v>1396.91</v>
+      </c>
+      <c r="C55" s="3">
+        <f t="shared" si="7"/>
+        <v>2639.039021841063</v>
+      </c>
+      <c r="D55" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E55" s="1">
+        <f t="shared" si="9"/>
+        <v>2639</v>
+      </c>
+      <c r="F55" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" s="4">
+        <v>1479.98</v>
+      </c>
+      <c r="C56" s="3">
+        <f t="shared" si="7"/>
+        <v>2490.9120393518829</v>
+      </c>
+      <c r="D56" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E56" s="1">
+        <f t="shared" si="9"/>
+        <v>2490</v>
+      </c>
+      <c r="F56" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="4">
+        <v>1567.98</v>
+      </c>
+      <c r="C57" s="3">
+        <f t="shared" si="7"/>
+        <v>2351.1141723746478</v>
+      </c>
+      <c r="D57" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E57" s="1">
+        <f t="shared" si="9"/>
+        <v>2351</v>
+      </c>
+      <c r="F57" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="4">
+        <v>1661.22</v>
+      </c>
+      <c r="C58" s="3">
+        <f t="shared" si="7"/>
+        <v>2219.1521893548115</v>
+      </c>
+      <c r="D58" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E58" s="1">
+        <f t="shared" si="9"/>
+        <v>2219</v>
+      </c>
+      <c r="F58" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="4">
+        <v>1760</v>
+      </c>
+      <c r="C59" s="3">
+        <f t="shared" si="7"/>
+        <v>2094.6022727272725</v>
+      </c>
+      <c r="D59" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E59" s="1">
+        <f t="shared" si="9"/>
+        <v>2094</v>
+      </c>
+      <c r="F59" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="4">
+        <v>1864.66</v>
+      </c>
+      <c r="C60" s="3">
+        <f t="shared" si="7"/>
+        <v>1977.0360280158311</v>
+      </c>
+      <c r="D60" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E60" s="1">
+        <f t="shared" si="9"/>
+        <v>1977</v>
+      </c>
+      <c r="F60" s="1" t="str">
+        <f t="shared" si="10"/>
+        <v>LONG</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="4">
-        <v>246.94</v>
-      </c>
-      <c r="C51" s="3">
-        <f>(1/B51)/($N$2*(1/$J$2))</f>
-        <v>14928.727626144004</v>
-      </c>
-      <c r="D51" s="1" t="str">
-        <f t="shared" si="8"/>
-        <v>LONG</v>
-      </c>
-      <c r="E51" s="1">
-        <f t="shared" si="9"/>
-        <v>14928</v>
-      </c>
-      <c r="F51" s="1" t="str">
+      <c r="B61" s="4">
+        <v>1975.53</v>
+      </c>
+      <c r="C61" s="3">
+        <f t="shared" si="7"/>
+        <v>1866.0815072410946</v>
+      </c>
+      <c r="D61" s="1" t="str">
+        <f t="shared" si="8"/>
+        <v>LONG</v>
+      </c>
+      <c r="E61" s="1">
+        <f t="shared" si="9"/>
+        <v>1866</v>
+      </c>
+      <c r="F61" s="1" t="str">
         <f t="shared" si="10"/>
         <v>LONG</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C24" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>